<commit_message>
fixing marginal effects (now conditional effects) to show both parts of hurdle, and contour graph for interaction
</commit_message>
<xml_diff>
--- a/doc/coef_values_v1_complete_only.xlsx
+++ b/doc/coef_values_v1_complete_only.xlsx
@@ -83,16 +83,16 @@
     <t>Zero-Inflated (Logistic)</t>
   </si>
   <si>
-    <t>GDP (dollars per capita)</t>
-  </si>
-  <si>
-    <t>ProMed Mentions (per capita)</t>
+    <t>ln(GDP [dollars per capita])</t>
+  </si>
+  <si>
+    <t>ln(ProMed Mentions [per capita])</t>
   </si>
   <si>
     <t>Livestock AB Consumption:GDP</t>
   </si>
   <si>
-    <t>Tourism - Inbound (per capita)</t>
+    <t>ln(Tourism - Inbound [per capita])</t>
   </si>
   <si>
     <t>Human AB Consumption (DDD)</t>
@@ -101,22 +101,22 @@
     <t>English Spoken (yes/no)</t>
   </si>
   <si>
-    <t>AB Exports (dollars per capita)</t>
-  </si>
-  <si>
-    <t>Migrant Population (per capita)</t>
+    <t>ln(AB Exports [dollars per capita])</t>
+  </si>
+  <si>
+    <t>ln(Migrant Population [per capita])</t>
   </si>
   <si>
     <t>Health Expenditure (% GDP)</t>
   </si>
   <si>
-    <t>Publication Bias Index (per capita)</t>
-  </si>
-  <si>
-    <t>Livestock AB Consumption (kg per capita)</t>
-  </si>
-  <si>
-    <t>Population</t>
+    <t>ln(Publication Bias Index [per capita])</t>
+  </si>
+  <si>
+    <t>Livestock AB Consumption [kg per capita)</t>
+  </si>
+  <si>
+    <t>ln(Population)</t>
   </si>
   <si>
     <t>29 (9.2-100)*</t>

</xml_diff>

<commit_message>
fix typo in label, update renv
</commit_message>
<xml_diff>
--- a/doc/coef_values_v1_complete_only.xlsx
+++ b/doc/coef_values_v1_complete_only.xlsx
@@ -83,16 +83,16 @@
     <t>Zero-Inflated (Logistic)</t>
   </si>
   <si>
-    <t>ln(GDP [dollars per capita])</t>
-  </si>
-  <si>
-    <t>ln(ProMed Mentions [per capita])</t>
+    <t>ln(GDP [dollars per cap.])</t>
+  </si>
+  <si>
+    <t>ln(ProMed Mentions [per cap.])</t>
   </si>
   <si>
     <t>Livestock AB Consumption:GDP</t>
   </si>
   <si>
-    <t>ln(Tourism - Inbound [per capita])</t>
+    <t>ln(Tourism - Inbound [per cap.])</t>
   </si>
   <si>
     <t>Human AB Consumption (DDD)</t>
@@ -101,19 +101,19 @@
     <t>English Spoken (yes/no)</t>
   </si>
   <si>
-    <t>ln(AB Exports [dollars per capita])</t>
-  </si>
-  <si>
-    <t>ln(Migrant Population [per capita])</t>
+    <t>ln(AB Exports [dollars per cap.])</t>
+  </si>
+  <si>
+    <t>ln(Migrant Population [per cap.])</t>
   </si>
   <si>
     <t>Health Expenditure (% GDP)</t>
   </si>
   <si>
-    <t>ln(Publication Bias Index [per capita])</t>
-  </si>
-  <si>
-    <t>Livestock AB Consumption [kg per capita)</t>
+    <t>ln(Publication Bias Index [per cap.])</t>
+  </si>
+  <si>
+    <t>Livestock AB Consumption (kg per cap.)</t>
   </si>
   <si>
     <t>ln(Population)</t>

</xml_diff>